<commit_message>
US 11 No Bigamy
</commit_message>
<xml_diff>
--- a/FinalProject/Excel Sheet/Team_DhruvalKunjNihirVyomYash_Report.xlsx
+++ b/FinalProject/Excel Sheet/Team_DhruvalKunjNihirVyomYash_Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kunj/Desktop/Stevens/CS555_Final_Project/FinalProject/Excel Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BB51CC-69EA-784D-9A52-EA09BFC329FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80E779D-CFD4-E34B-BA97-8704D5FB1326}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15760" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="265">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2353,8 +2353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A11" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3253,7 +3253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView zoomScale="105" zoomScaleNormal="157" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="157" workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -3939,7 +3939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+    <sheetView zoomScale="113" workbookViewId="0">
       <selection activeCell="G2" sqref="G2:H4"/>
     </sheetView>
   </sheetViews>
@@ -4405,10 +4405,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:Q29"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4478,9 +4478,15 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" t="s">
+        <v>177</v>
+      </c>
       <c r="F2" s="21"/>
       <c r="K2" s="18"/>
       <c r="L2" s="20"/>
@@ -4489,35 +4495,46 @@
       <c r="P2" s="20"/>
       <c r="Q2" s="18"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="4"/>
+    <row r="3" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="B3"/>
+      <c r="F3" s="21"/>
       <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
+      <c r="L3" s="20"/>
       <c r="M3" s="18"/>
       <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
+      <c r="P3" s="20"/>
       <c r="Q3" s="18"/>
     </row>
-    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="H4" s="21"/>
-      <c r="L4" s="20"/>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" t="s">
+        <v>177</v>
+      </c>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
       <c r="M4" s="18"/>
+      <c r="O4" s="18"/>
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="4"/>
+      <c r="H5" s="21"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
+      <c r="B6" s="5"/>
       <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.15">
@@ -4559,11 +4576,6 @@
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
@@ -4579,6 +4591,11 @@
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
@@ -4600,21 +4617,26 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="23" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="B23" s="5" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="24" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="B24" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B24" s="5"/>
-    </row>
-    <row r="25" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="B25" s="5" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B25" s="5"/>
+    </row>
+    <row r="26" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="B26" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="B29" s="5" t="s">
+    <row r="30" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="B30" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4877,8 +4899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Updates for sprint - 2
</commit_message>
<xml_diff>
--- a/FinalProject/Excel Sheet/Team_DhruvalKunjNihirVyomYash_Report.xlsx
+++ b/FinalProject/Excel Sheet/Team_DhruvalKunjNihirVyomYash_Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kunj/Desktop/Stevens/CS555_Final_Project/FinalProject/Excel Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80E779D-CFD4-E34B-BA97-8704D5FB1326}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDAFDEE-62AA-3142-A7CC-C8ABAE5CDB67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="266">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -752,21 +752,9 @@
     <t>test_us_18_Siblings_should_not_marry</t>
   </si>
   <si>
-    <t>33-82</t>
-  </si>
-  <si>
-    <t>92-125</t>
-  </si>
-  <si>
     <t>Act Size</t>
   </si>
   <si>
-    <t>178-223</t>
-  </si>
-  <si>
-    <t>234-284</t>
-  </si>
-  <si>
     <t>us03_birth_before_death</t>
   </si>
   <si>
@@ -794,12 +782,6 @@
     <t>us_22_unique_ids</t>
   </si>
   <si>
-    <t>135-170</t>
-  </si>
-  <si>
-    <t>64-86</t>
-  </si>
-  <si>
     <t>test_us_22_unique_ids</t>
   </si>
   <si>
@@ -836,24 +818,6 @@
     <t>Merge conflicting branch</t>
   </si>
   <si>
-    <t>295-328</t>
-  </si>
-  <si>
-    <t>338-386</t>
-  </si>
-  <si>
-    <t>397-451</t>
-  </si>
-  <si>
-    <t>461-509</t>
-  </si>
-  <si>
-    <t>511-540</t>
-  </si>
-  <si>
-    <t>549-573</t>
-  </si>
-  <si>
     <t>93-99</t>
   </si>
   <si>
@@ -864,6 +828,45 @@
   </si>
   <si>
     <t>778-816</t>
+  </si>
+  <si>
+    <t>34-83</t>
+  </si>
+  <si>
+    <t>93-126</t>
+  </si>
+  <si>
+    <t>65-87</t>
+  </si>
+  <si>
+    <t>136-171</t>
+  </si>
+  <si>
+    <t>550-574</t>
+  </si>
+  <si>
+    <t>512-541</t>
+  </si>
+  <si>
+    <t>296-329</t>
+  </si>
+  <si>
+    <t>339-387</t>
+  </si>
+  <si>
+    <t>398-452</t>
+  </si>
+  <si>
+    <t>462-510</t>
+  </si>
+  <si>
+    <t>179-224</t>
+  </si>
+  <si>
+    <t>235-285</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -3253,8 +3256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView zoomScale="105" zoomScaleNormal="157" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3297,7 +3300,7 @@
         <v>14</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H1" s="10" t="s">
         <v>15</v>
@@ -3359,7 +3362,7 @@
         <v>207</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>227</v>
+        <v>253</v>
       </c>
       <c r="O2" s="18" t="s">
         <v>209</v>
@@ -3420,7 +3423,7 @@
         <v>208</v>
       </c>
       <c r="M4" s="18" t="s">
-        <v>228</v>
+        <v>254</v>
       </c>
       <c r="O4" s="17" t="s">
         <v>209</v>
@@ -3469,22 +3472,22 @@
         <v>205</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="O6" s="17" t="s">
         <v>209</v>
       </c>
       <c r="P6" s="17" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="Q6" s="17" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.15">
@@ -3527,19 +3530,19 @@
         <v>206</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="O8" s="17" t="s">
         <v>209</v>
       </c>
       <c r="P8" s="17" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="Q8" s="17" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.15">
@@ -3585,7 +3588,7 @@
         <v>223</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="O10" s="17" t="s">
         <v>209</v>
@@ -3594,7 +3597,7 @@
         <v>225</v>
       </c>
       <c r="Q10" s="17" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.15">
@@ -3640,7 +3643,7 @@
         <v>224</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="O12" s="17" t="s">
         <v>209</v>
@@ -3649,7 +3652,7 @@
         <v>226</v>
       </c>
       <c r="Q12" s="17" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.15">
@@ -3692,19 +3695,19 @@
         <v>206</v>
       </c>
       <c r="L14" s="18" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="M14" s="18" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="O14" s="17" t="s">
         <v>209</v>
       </c>
       <c r="P14" s="18" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="Q14" s="18" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.15">
@@ -3751,19 +3754,19 @@
         <v>206</v>
       </c>
       <c r="L16" s="18" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="M16" s="17" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="O16" s="17" t="s">
         <v>209</v>
       </c>
       <c r="P16" s="18" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="Q16" s="17" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.15">
@@ -3806,19 +3809,19 @@
         <v>206</v>
       </c>
       <c r="L18" s="17" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="M18" s="17" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="O18" s="17" t="s">
         <v>209</v>
       </c>
       <c r="P18" s="17" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="Q18" s="17" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.15">
@@ -3861,19 +3864,19 @@
         <v>206</v>
       </c>
       <c r="L20" s="17" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="M20" s="17" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="O20" s="17" t="s">
         <v>209</v>
       </c>
       <c r="P20" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q20" s="17" t="s">
         <v>249</v>
-      </c>
-      <c r="Q20" s="17" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="14" x14ac:dyDescent="0.15">
@@ -3891,12 +3894,12 @@
     </row>
     <row r="26" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="B26" s="1" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="B27" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="14" x14ac:dyDescent="0.15">
@@ -3906,12 +3909,12 @@
     </row>
     <row r="30" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="B30" s="1" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="B31" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -3939,8 +3942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H4"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4044,7 +4047,7 @@
         <v>215</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>230</v>
+        <v>263</v>
       </c>
       <c r="O2" s="18" t="s">
         <v>209</v>
@@ -4104,7 +4107,7 @@
         <v>220</v>
       </c>
       <c r="M4" s="18" t="s">
-        <v>231</v>
+        <v>264</v>
       </c>
       <c r="O4" s="17" t="s">
         <v>209</v>
@@ -4144,6 +4147,9 @@
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
+      <c r="I6" s="7" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7" s="4"/>
@@ -4174,6 +4180,9 @@
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
+      <c r="I8" s="7" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
@@ -4203,6 +4212,9 @@
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
+      <c r="I10" s="7" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A11" s="4"/>
@@ -4232,6 +4244,9 @@
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
+      <c r="I12" s="7" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
@@ -4261,6 +4276,9 @@
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
+      <c r="I14" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="L14" s="18"/>
       <c r="M14" s="18"/>
       <c r="O14" s="18"/>
@@ -4300,15 +4318,18 @@
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I16" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
         <v>123</v>
       </c>
@@ -4329,15 +4350,18 @@
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I18" s="7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>125</v>
       </c>
@@ -4358,26 +4382,29 @@
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
-    </row>
-    <row r="23" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="I20" s="7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B23" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B24" s="5"/>
     </row>
-    <row r="25" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B25" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B29" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="28" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="B30" s="24" t="s">
         <v>218</v>
       </c>
@@ -4407,7 +4434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="88" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -5221,7 +5248,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>133</v>
       </c>

</xml_diff>

<commit_message>
Excelsheet updated with my detail
</commit_message>
<xml_diff>
--- a/FinalProject/Excel Sheet/Team_DhruvalKunjNihirVyomYash_Report.xlsx
+++ b/FinalProject/Excel Sheet/Team_DhruvalKunjNihirVyomYash_Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kunj/Desktop/Stevens/CS555_Final_Project/FinalProject/Excel Sheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhruval\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDAFDEE-62AA-3142-A7CC-C8ABAE5CDB67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCA82E2D-6609-43CB-BB41-61DDDECD19FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="274">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -867,6 +867,30 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>us15_fewer_than_15_siblings()</t>
+  </si>
+  <si>
+    <t>us20_aunts_and_uncles()</t>
+  </si>
+  <si>
+    <t>585-615</t>
+  </si>
+  <si>
+    <t>626-684</t>
+  </si>
+  <si>
+    <t>test_us15_fewer_than_15_siblings()</t>
+  </si>
+  <si>
+    <t>test_us20_aunts_and_uncles()</t>
+  </si>
+  <si>
+    <t>117-123</t>
+  </si>
+  <si>
+    <t>125-131</t>
   </si>
 </sst>
 </file>
@@ -1176,7 +1200,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42409</c:v>
@@ -1235,7 +1259,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2216,16 +2240,16 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" customWidth="1"/>
+    <col min="5" max="5" width="47.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -2242,7 +2266,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>177</v>
       </c>
@@ -2259,7 +2283,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -2276,7 +2300,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>183</v>
       </c>
@@ -2293,7 +2317,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>188</v>
       </c>
@@ -2310,7 +2334,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>191</v>
       </c>
@@ -2327,7 +2351,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>29</v>
       </c>
@@ -2356,20 +2380,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:D23"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.1640625" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
@@ -2386,7 +2410,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2403,7 +2427,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2420,7 +2444,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2437,7 +2461,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2454,7 +2478,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2471,7 +2495,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2488,7 +2512,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2505,7 +2529,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2522,7 +2546,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2539,7 +2563,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2556,7 +2580,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2573,7 +2597,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2590,7 +2614,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2607,7 +2631,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2624,7 +2648,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2641,7 +2665,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2658,7 +2682,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2671,11 +2695,11 @@
       <c r="D18" t="s">
         <v>183</v>
       </c>
-      <c r="E18" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E18" s="21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2688,11 +2712,11 @@
       <c r="D19" t="s">
         <v>183</v>
       </c>
-      <c r="E19" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E19" s="21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2709,7 +2733,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2726,7 +2750,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2740,7 +2764,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2754,7 +2778,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2768,7 +2792,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2782,7 +2806,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2796,7 +2820,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3</v>
       </c>
@@ -2810,7 +2834,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3</v>
       </c>
@@ -2824,7 +2848,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3</v>
       </c>
@@ -2838,7 +2862,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
@@ -2852,7 +2876,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2866,7 +2890,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2880,7 +2904,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -2894,7 +2918,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2908,7 +2932,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2922,7 +2946,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2936,7 +2960,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2950,7 +2974,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>4</v>
       </c>
@@ -2964,7 +2988,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>4</v>
       </c>
@@ -2978,7 +3002,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>4</v>
       </c>
@@ -2992,7 +3016,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3029,47 +3053,47 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="7"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>154</v>
       </c>
@@ -3092,7 +3116,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -3106,7 +3130,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>156</v>
       </c>
@@ -3127,7 +3151,7 @@
         <v>32.680851063829785</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>157</v>
       </c>
@@ -3144,7 +3168,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>158</v>
       </c>
@@ -3157,7 +3181,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>159</v>
       </c>
@@ -3185,17 +3209,17 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="2"/>
+    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3215,7 +3239,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>42409</v>
       </c>
@@ -3226,7 +3250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>42430</v>
       </c>
@@ -3260,27 +3284,27 @@
       <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.81640625" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.83203125" style="17" customWidth="1"/>
-    <col min="15" max="15" width="19.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.81640625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="19.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1796875" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3327,7 +3351,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>108</v>
       </c>
@@ -3374,7 +3398,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="4"/>
@@ -3388,7 +3412,7 @@
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
     </row>
-    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>110</v>
       </c>
@@ -3435,7 +3459,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="4"/>
@@ -3443,7 +3467,7 @@
       <c r="H5" s="21"/>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>133</v>
       </c>
@@ -3490,7 +3514,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -3498,7 +3522,7 @@
       <c r="H7" s="21"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>128</v>
       </c>
@@ -3545,7 +3569,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -3553,7 +3577,7 @@
       <c r="H9" s="21"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>122</v>
       </c>
@@ -3600,7 +3624,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -3608,7 +3632,7 @@
       <c r="H11" s="21"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>124</v>
       </c>
@@ -3655,7 +3679,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -3663,7 +3687,7 @@
       <c r="H13" s="21"/>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>109</v>
       </c>
@@ -3710,7 +3734,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -3722,7 +3746,7 @@
       <c r="O15" s="18"/>
       <c r="Q15" s="18"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>111</v>
       </c>
@@ -3769,7 +3793,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -3777,7 +3801,7 @@
       <c r="H17" s="21"/>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>113</v>
       </c>
@@ -3824,7 +3848,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -3832,7 +3856,7 @@
       <c r="H19" s="21"/>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>114</v>
       </c>
@@ -3879,40 +3903,40 @@
         <v>249</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B24" s="5"/>
     </row>
-    <row r="25" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>248</v>
       </c>
@@ -3942,30 +3966,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView zoomScale="113" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.81640625" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.83203125" style="17" customWidth="1"/>
-    <col min="15" max="15" width="19.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.1640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.81640625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="19.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1796875" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4012,7 +4036,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>112</v>
       </c>
@@ -4059,7 +4083,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="4"/>
@@ -4072,7 +4096,7 @@
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
     </row>
-    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>116</v>
       </c>
@@ -4119,14 +4143,14 @@
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>141</v>
       </c>
@@ -4151,7 +4175,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -4159,7 +4183,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>144</v>
       </c>
@@ -4184,14 +4208,14 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>119</v>
       </c>
@@ -4216,14 +4240,14 @@
         <v>205</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>120</v>
       </c>
@@ -4248,14 +4272,14 @@
         <v>205</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>121</v>
       </c>
@@ -4266,7 +4290,7 @@
         <v>183</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="E14">
         <v>35</v>
@@ -4274,18 +4298,35 @@
       <c r="F14">
         <v>60</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="G14" s="21">
+        <v>30</v>
+      </c>
+      <c r="H14" s="21">
+        <v>35</v>
+      </c>
       <c r="I14" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="K14" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="L14" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="M14" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="O14" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="P14" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q14" s="18" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -4297,7 +4338,7 @@
       <c r="P15" s="18"/>
       <c r="Q15" s="18"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>126</v>
       </c>
@@ -4308,7 +4349,7 @@
         <v>183</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="E16">
         <v>45</v>
@@ -4316,20 +4357,42 @@
       <c r="F16">
         <v>70</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="G16" s="21">
+        <v>58</v>
+      </c>
+      <c r="H16" s="21">
+        <v>45</v>
+      </c>
       <c r="I16" s="7" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="K16" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="L16" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="M16" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="O16" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="P16" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q16" s="18" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>123</v>
       </c>
@@ -4354,14 +4417,14 @@
         <v>265</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>125</v>
       </c>
@@ -4386,25 +4449,25 @@
         <v>265</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B24" s="5"/>
     </row>
-    <row r="25" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B30" s="24" t="s">
         <v>218</v>
       </c>
@@ -4426,7 +4489,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4438,26 +4501,26 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.81640625" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.83203125" style="17" customWidth="1"/>
-    <col min="15" max="15" width="19.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.81640625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="19.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1796875" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4504,7 +4567,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>117</v>
       </c>
@@ -4522,7 +4585,7 @@
       <c r="P2" s="20"/>
       <c r="Q2" s="18"/>
     </row>
-    <row r="3" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="B3"/>
       <c r="F3" s="21"/>
       <c r="K3" s="18"/>
@@ -4532,7 +4595,7 @@
       <c r="P3" s="20"/>
       <c r="Q3" s="18"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -4549,7 +4612,7 @@
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
     </row>
-    <row r="5" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -4559,52 +4622,52 @@
       <c r="P5" s="18"/>
       <c r="Q5" s="18"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -4614,7 +4677,7 @@
       <c r="P15" s="18"/>
       <c r="Q15" s="18"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -4624,45 +4687,45 @@
       <c r="P16" s="18"/>
       <c r="Q16" s="18"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="24" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B25" s="5"/>
     </row>
-    <row r="26" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
         <v>27</v>
       </c>
@@ -4695,26 +4758,26 @@
       <selection activeCell="A2" sqref="A2:C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.81640625" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.83203125" style="17" customWidth="1"/>
-    <col min="15" max="15" width="19.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.81640625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="19.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1796875" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4761,7 +4824,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -4773,7 +4836,7 @@
       <c r="P2" s="20"/>
       <c r="Q2" s="18"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="4"/>
@@ -4784,7 +4847,7 @@
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
     </row>
-    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -4794,52 +4857,52 @@
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -4849,7 +4912,7 @@
       <c r="P14" s="18"/>
       <c r="Q14" s="18"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -4859,45 +4922,45 @@
       <c r="P15" s="18"/>
       <c r="Q15" s="18"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="23" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B24" s="5"/>
     </row>
-    <row r="25" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
         <v>27</v>
       </c>
@@ -4930,13 +4993,13 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>106</v>
       </c>
@@ -4950,7 +5013,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -4961,7 +5024,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>108</v>
       </c>
@@ -4975,7 +5038,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -4986,7 +5049,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -5000,7 +5063,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -5011,7 +5074,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -5025,7 +5088,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -5036,7 +5099,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -5047,7 +5110,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -5058,7 +5121,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -5072,7 +5135,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -5083,7 +5146,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -5094,7 +5157,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -5105,7 +5168,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>120</v>
       </c>
@@ -5116,7 +5179,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>121</v>
       </c>
@@ -5127,7 +5190,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>122</v>
       </c>
@@ -5138,7 +5201,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -5149,7 +5212,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>124</v>
       </c>
@@ -5160,7 +5223,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>125</v>
       </c>
@@ -5171,7 +5234,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -5182,7 +5245,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -5193,7 +5256,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>128</v>
       </c>
@@ -5204,7 +5267,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -5215,7 +5278,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>130</v>
       </c>
@@ -5226,7 +5289,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -5237,7 +5300,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>132</v>
       </c>
@@ -5248,7 +5311,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>133</v>
       </c>
@@ -5259,7 +5322,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -5270,7 +5333,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>135</v>
       </c>
@@ -5281,7 +5344,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>136</v>
       </c>
@@ -5292,7 +5355,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>137</v>
       </c>
@@ -5303,7 +5366,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>138</v>
       </c>
@@ -5314,7 +5377,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>139</v>
       </c>
@@ -5325,7 +5388,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>140</v>
       </c>
@@ -5336,7 +5399,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>141</v>
       </c>
@@ -5347,7 +5410,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -5358,7 +5421,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -5369,7 +5432,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>144</v>
       </c>
@@ -5380,7 +5443,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>145</v>
       </c>
@@ -5391,7 +5454,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>146</v>
       </c>
@@ -5402,7 +5465,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>147</v>
       </c>
@@ -5413,7 +5476,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
Update in excel done
</commit_message>
<xml_diff>
--- a/FinalProject/Excel Sheet/Team_DhruvalKunjNihirVyomYash_Report.xlsx
+++ b/FinalProject/Excel Sheet/Team_DhruvalKunjNihirVyomYash_Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nihir\Desktop\cs590\assignment1\CS555_Final_Project\FinalProject\Excel Sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhruval\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768F7877-9A23-478C-B0A5-CC6C994DF552}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39DCDB4-2A72-4175-9186-04BD5512EDD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="321">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1008,6 +1008,30 @@
   </si>
   <si>
     <t>us34_list_living_married()</t>
+  </si>
+  <si>
+    <t>us24_Unique_families_by_spouses()</t>
+  </si>
+  <si>
+    <t>us32_list_multiple_births()</t>
+  </si>
+  <si>
+    <t>1262-1322</t>
+  </si>
+  <si>
+    <t>1215-1252</t>
+  </si>
+  <si>
+    <t>test_us24_Unique_families_by_spouses()</t>
+  </si>
+  <si>
+    <t>test_us32_list_multiple_births()</t>
+  </si>
+  <si>
+    <t>237-243</t>
+  </si>
+  <si>
+    <t>152-158</t>
   </si>
 </sst>
 </file>
@@ -2376,13 +2400,13 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="47.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" customWidth="1"/>
+    <col min="5" max="5" width="47.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2516,17 +2540,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.125" customWidth="1"/>
-    <col min="2" max="2" width="7.625" customWidth="1"/>
-    <col min="3" max="3" width="26.125" customWidth="1"/>
-    <col min="4" max="4" width="6.625" customWidth="1"/>
-    <col min="5" max="5" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.08984375" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="26.08984375" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -3001,8 +3025,8 @@
       <c r="D28" t="s">
         <v>183</v>
       </c>
-      <c r="E28" t="s">
-        <v>217</v>
+      <c r="E28" s="21" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -3018,8 +3042,8 @@
       <c r="D29" t="s">
         <v>183</v>
       </c>
-      <c r="E29" t="s">
-        <v>217</v>
+      <c r="E29" s="21" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -3035,7 +3059,7 @@
       <c r="D30" t="s">
         <v>191</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="21" t="s">
         <v>204</v>
       </c>
     </row>
@@ -3070,7 +3094,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -3084,7 +3108,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4</v>
       </c>
@@ -3098,7 +3122,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -3112,7 +3136,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>4</v>
       </c>
@@ -3126,7 +3150,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>4</v>
       </c>
@@ -3140,7 +3164,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3153,8 +3177,11 @@
       <c r="D38" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" s="21" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>4</v>
       </c>
@@ -3167,8 +3194,11 @@
       <c r="D39" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" s="21" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>4</v>
       </c>
@@ -3182,7 +3212,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3219,14 +3249,14 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="7"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="7"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -3383,14 +3413,14 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="2"/>
+    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="7.08984375" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -3484,24 +3514,24 @@
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.375" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.875" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.90625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.90625" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.875" style="17" customWidth="1"/>
-    <col min="15" max="15" width="19.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.125" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.90625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="19.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.08984375" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
@@ -3551,7 +3581,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>108</v>
       </c>
@@ -3612,7 +3642,7 @@
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
     </row>
-    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>110</v>
       </c>
@@ -4177,26 +4207,26 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.375" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.875" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.90625" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.875" style="17" customWidth="1"/>
-    <col min="15" max="15" width="19.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.125" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.125" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.90625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="19.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.08984375" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.08984375" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
@@ -4246,7 +4276,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>112</v>
       </c>
@@ -4306,7 +4336,7 @@
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
     </row>
-    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>116</v>
       </c>
@@ -4603,7 +4633,7 @@
         <v>183</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="E14">
         <v>35</v>
@@ -4665,7 +4695,7 @@
         <v>183</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="E16">
         <v>45</v>
@@ -4854,7 +4884,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B30" s="24" t="s">
         <v>218</v>
       </c>
@@ -4884,27 +4914,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView zoomScale="110" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.375" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.875" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.90625" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.875" style="17" customWidth="1"/>
-    <col min="15" max="15" width="19.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.90625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="19.453125" style="17" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="32" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.125" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.08984375" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
@@ -4954,7 +4984,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>117</v>
       </c>
@@ -4998,7 +5028,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -5068,7 +5098,7 @@
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
     </row>
-    <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>134</v>
       </c>
@@ -5191,14 +5221,41 @@
       <c r="C8" t="s">
         <v>183</v>
       </c>
-      <c r="D8" t="s">
-        <v>217</v>
+      <c r="D8" s="21" t="s">
+        <v>204</v>
       </c>
       <c r="E8">
         <v>20</v>
       </c>
       <c r="F8">
         <v>67</v>
+      </c>
+      <c r="G8">
+        <v>37</v>
+      </c>
+      <c r="H8">
+        <v>25</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="L8" s="17" t="s">
+        <v>313</v>
+      </c>
+      <c r="M8" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="O8" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="P8" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="Q8" s="18" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -5211,14 +5268,41 @@
       <c r="C9" t="s">
         <v>183</v>
       </c>
-      <c r="D9" t="s">
-        <v>217</v>
+      <c r="D9" s="21" t="s">
+        <v>204</v>
       </c>
       <c r="E9">
         <v>43</v>
       </c>
       <c r="F9">
         <v>80</v>
+      </c>
+      <c r="G9">
+        <v>60</v>
+      </c>
+      <c r="H9">
+        <v>45</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="M9" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="O9" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="P9" s="18" t="s">
+        <v>318</v>
+      </c>
+      <c r="Q9" s="18" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -5240,6 +5324,7 @@
       <c r="F10">
         <v>30</v>
       </c>
+      <c r="K10" s="18"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -5267,11 +5352,11 @@
       <c r="C12" s="4"/>
       <c r="G12">
         <f>SUM(G2:G11)</f>
-        <v>176</v>
+        <v>273</v>
       </c>
       <c r="H12">
         <f>SUM(H2:H11)</f>
-        <v>225</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -5364,6 +5449,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5375,23 +5461,23 @@
       <selection activeCell="A2" sqref="A2:C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.375" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.875" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.90625" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.875" style="17" customWidth="1"/>
-    <col min="15" max="15" width="19.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.125" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.90625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="19.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.08984375" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
@@ -5441,7 +5527,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -5464,7 +5550,7 @@
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
     </row>
-    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -5610,10 +5696,10 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -5630,7 +5716,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -5641,7 +5727,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>108</v>
       </c>
@@ -5655,7 +5741,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -5666,7 +5752,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -5680,7 +5766,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -5691,7 +5777,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -5705,7 +5791,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -5716,7 +5802,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -5727,7 +5813,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -5738,7 +5824,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -5752,7 +5838,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -5763,7 +5849,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -5774,7 +5860,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -5785,7 +5871,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>120</v>
       </c>
@@ -5796,7 +5882,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>121</v>
       </c>
@@ -5807,7 +5893,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>122</v>
       </c>
@@ -5818,7 +5904,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -5829,7 +5915,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>124</v>
       </c>
@@ -5840,7 +5926,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>125</v>
       </c>
@@ -5851,7 +5937,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -5862,7 +5948,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -5873,7 +5959,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>128</v>
       </c>
@@ -5887,7 +5973,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -5898,7 +5984,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>130</v>
       </c>
@@ -5909,7 +5995,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -5920,7 +6006,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="126" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>132</v>
       </c>
@@ -5931,7 +6017,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>133</v>
       </c>
@@ -5945,7 +6031,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -5956,7 +6042,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>135</v>
       </c>
@@ -5967,7 +6053,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>136</v>
       </c>
@@ -5978,7 +6064,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>137</v>
       </c>
@@ -5989,7 +6075,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>138</v>
       </c>
@@ -6000,7 +6086,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>139</v>
       </c>
@@ -6011,7 +6097,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>140</v>
       </c>
@@ -6022,7 +6108,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>141</v>
       </c>
@@ -6036,7 +6122,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -6047,7 +6133,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -6058,7 +6144,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>144</v>
       </c>
@@ -6072,7 +6158,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>145</v>
       </c>
@@ -6083,7 +6169,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>146</v>
       </c>
@@ -6094,7 +6180,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>147</v>
       </c>
@@ -6105,7 +6191,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>148</v>
       </c>

</xml_diff>